<commit_message>
testing for hamming calculations
</commit_message>
<xml_diff>
--- a/c880 and c3540 io.xlsx
+++ b/c880 and c3540 io.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TheFolder/Documents/ECE 459/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtvar\ECE459\Project\ECE459PUF-Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887CD723-C713-654D-A1D2-362DB049DEC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2331E966-CA07-44AF-8ECC-7AA13B71ABE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14760" xr2:uid="{0905E3DD-815B-2B4C-A5D9-53817CD19009}"/>
+    <workbookView xWindow="20370" yWindow="-9015" windowWidth="29040" windowHeight="16440" xr2:uid="{0905E3DD-815B-2B4C-A5D9-53817CD19009}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>C3540</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>00010111101000110101000100</t>
+  </si>
+  <si>
+    <t>Correct Key:</t>
+  </si>
+  <si>
+    <t>110100100</t>
+  </si>
+  <si>
+    <t>correct output</t>
   </si>
 </sst>
 </file>
@@ -536,194 +545,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347F5D6A-048F-8D41-B15C-C4584D1C6AF9}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>